<commit_message>
Getting closer to understanding
</commit_message>
<xml_diff>
--- a/Excel-BI-Excel-Challenge-436.xlsx
+++ b/Excel-BI-Excel-Challenge-436.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{27646988-AD42-4DB1-BB6C-B0121AE541EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A986209-C765-4242-9055-3A9F868FD63D}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{27646988-AD42-4DB1-BB6C-B0121AE541EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5EB7A6F-451A-46CE-BFA7-BB23476A460F}"/>
   <bookViews>
-    <workbookView xWindow="57660" yWindow="3195" windowWidth="21600" windowHeight="11235" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="11" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>FROM:</t>
   </si>
@@ -145,6 +147,18 @@
   </si>
   <si>
     <t>Reference Info Card</t>
+  </si>
+  <si>
+    <t>This is clever. He is building the number from the back.</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>append 1</t>
+  </si>
+  <si>
+    <t>Column</t>
   </si>
 </sst>
 </file>
@@ -384,7 +398,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -398,7 +412,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -420,7 +433,21 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -653,27 +680,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="totalRow" dxfId="16"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="14"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="12"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="11"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="10"/>
+      <tableStyleElement type="pageFieldValues" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="lastColumn" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1126,7 +1153,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1418,10 +1445,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35:W61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E17" t="str">
         <v>321</v>
       </c>
@@ -1529,7 +1556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21:E26">_xlfn.LET(_xlpm.n,3,_xlpm.s,_xlfn.SEQUENCE(,_xlpm.n),_xlfn.REDUCE(_xlfn.TOCOL(_xlpm.s),_xlfn.DROP(_xlpm.s,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.TOCOL(_xlfn.IFS(ISERR(FIND(_xlpm.s,_xlpm.a)),_xlpm.a&amp;_xlpm.s),3))))</f>
         <v>123</v>
@@ -1543,8 +1570,15 @@
       <c r="J21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="str" cm="1">
+        <f t="array" ref="N21:N23">M21:M23&amp;2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E22" t="str">
         <v>132</v>
       </c>
@@ -1557,8 +1591,14 @@
       <c r="J22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E23" t="str">
         <v>213</v>
       </c>
@@ -1571,23 +1611,1138 @@
       <c r="J23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23" t="str">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E24" t="str">
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E25" t="str">
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E26" t="str">
         <v>321</v>
       </c>
     </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="str" cm="1">
+        <f t="array" ref="A29:C31">_xlfn.LET(_xlpm.n,3,_xlpm.s,_xlfn.SEQUENCE(,_xlpm.n),_xlfn.REDUCE(_xlfn.TOCOL(_xlpm.s),_xlfn.DROP(_xlpm.s,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a&amp;_xlpm.s)))</f>
+        <v>111</v>
+      </c>
+      <c r="B29" t="str">
+        <v>122</v>
+      </c>
+      <c r="C29" t="str">
+        <v>133</v>
+      </c>
+      <c r="E29" t="str" cm="1">
+        <f t="array" ref="E29:E55">_xlfn.LET(_xlpm.n,3,_xlpm.s,_xlfn.SEQUENCE(,_xlpm.n),_xlfn.REDUCE(_xlfn.TOCOL(_xlpm.s),_xlfn.DROP(_xlpm.s,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.TOCOL(_xlpm.a&amp;_xlpm.s))))</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <v>211</v>
+      </c>
+      <c r="B30" t="str">
+        <v>222</v>
+      </c>
+      <c r="C30" t="str">
+        <v>233</v>
+      </c>
+      <c r="E30" t="str">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <v>311</v>
+      </c>
+      <c r="B31" t="str">
+        <v>322</v>
+      </c>
+      <c r="C31" t="str">
+        <v>333</v>
+      </c>
+      <c r="E31" t="str">
+        <v>113</v>
+      </c>
+      <c r="I31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E32" t="str">
+        <v>121</v>
+      </c>
+      <c r="H32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E33" t="str">
+        <v>122</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E34" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E35" t="str">
+        <v>131</v>
+      </c>
+      <c r="J35" t="str" cm="1">
+        <f t="array" ref="J35:J61">_xlfn.LET(_xlpm.n,3,_xlpm.s,_xlfn.SEQUENCE(,_xlpm.n),_xlfn.REDUCE(_xlfn.TOCOL(_xlpm.s),_xlfn.DROP(_xlpm.s,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.TOCOL(_xlpm.a&amp;_xlpm.s))))</f>
+        <v>111</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="str" cm="1">
+        <f t="array" ref="M35:O37">L35:L37&amp;L33:N33</f>
+        <v>11</v>
+      </c>
+      <c r="N35" t="str">
+        <v>12</v>
+      </c>
+      <c r="O35" t="str">
+        <v>13</v>
+      </c>
+      <c r="R35" t="str" cm="1">
+        <f t="array" ref="R35:R43">_xlfn.TOCOL(_xlfn.ANCHORARRAY(M35))</f>
+        <v>11</v>
+      </c>
+      <c r="S35" t="str" cm="1">
+        <f t="array" ref="S35:U43">_xlfn.ANCHORARRAY(R35)&amp;L33:N33</f>
+        <v>111</v>
+      </c>
+      <c r="T35" t="str">
+        <v>112</v>
+      </c>
+      <c r="U35" t="str">
+        <v>113</v>
+      </c>
+      <c r="W35" t="str" cm="1">
+        <f t="array" ref="W35:W61">_xlfn.TOCOL(_xlfn.ANCHORARRAY(S35))</f>
+        <v>111</v>
+      </c>
+      <c r="X35" cm="1">
+        <f t="array" ref="X35:Z35">FIND($L$33:$N$33,W35)</f>
+        <v>1</v>
+      </c>
+      <c r="Y35" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z35" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA35" t="b">
+        <f>ISERR(X35)</f>
+        <v>0</v>
+      </c>
+      <c r="AB35" t="b">
+        <f t="shared" ref="AB35:AC35" si="0">ISERR(Y35)</f>
+        <v>1</v>
+      </c>
+      <c r="AC35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E36" t="str">
+        <v>132</v>
+      </c>
+      <c r="J36" t="str">
+        <v>112</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36" t="str">
+        <v>21</v>
+      </c>
+      <c r="N36" t="str">
+        <v>22</v>
+      </c>
+      <c r="O36" t="str">
+        <v>23</v>
+      </c>
+      <c r="R36" t="str">
+        <v>12</v>
+      </c>
+      <c r="S36" t="str">
+        <v>121</v>
+      </c>
+      <c r="T36" t="str">
+        <v>122</v>
+      </c>
+      <c r="U36" t="str">
+        <v>123</v>
+      </c>
+      <c r="W36" t="str">
+        <v>112</v>
+      </c>
+      <c r="X36" cm="1">
+        <f t="array" ref="X36:Z36">FIND($L$33:$N$33,W36)</f>
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <v>3</v>
+      </c>
+      <c r="Z36" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA36" t="b">
+        <f t="shared" ref="AA36:AA61" si="1">ISERR(X36)</f>
+        <v>0</v>
+      </c>
+      <c r="AB36" t="b">
+        <f t="shared" ref="AB36:AB61" si="2">ISERR(Y36)</f>
+        <v>0</v>
+      </c>
+      <c r="AC36" t="b">
+        <f t="shared" ref="AC36:AC61" si="3">ISERR(Z36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E37" t="str">
+        <v>133</v>
+      </c>
+      <c r="J37" t="str">
+        <v>113</v>
+      </c>
+      <c r="L37">
+        <v>3</v>
+      </c>
+      <c r="M37" t="str">
+        <v>31</v>
+      </c>
+      <c r="N37" t="str">
+        <v>32</v>
+      </c>
+      <c r="O37" t="str">
+        <v>33</v>
+      </c>
+      <c r="R37" t="str">
+        <v>13</v>
+      </c>
+      <c r="S37" t="str">
+        <v>131</v>
+      </c>
+      <c r="T37" t="str">
+        <v>132</v>
+      </c>
+      <c r="U37" t="str">
+        <v>133</v>
+      </c>
+      <c r="W37" t="str">
+        <v>113</v>
+      </c>
+      <c r="X37" cm="1">
+        <f t="array" ref="X37:Z37">FIND($L$33:$N$33,W37)</f>
+        <v>1</v>
+      </c>
+      <c r="Y37" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z37">
+        <v>3</v>
+      </c>
+      <c r="AA37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB37" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC37" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E38" t="str">
+        <v>211</v>
+      </c>
+      <c r="J38" t="str">
+        <v>121</v>
+      </c>
+      <c r="R38" t="str">
+        <v>21</v>
+      </c>
+      <c r="S38" t="str">
+        <v>211</v>
+      </c>
+      <c r="T38" t="str">
+        <v>212</v>
+      </c>
+      <c r="U38" t="str">
+        <v>213</v>
+      </c>
+      <c r="W38" t="str">
+        <v>121</v>
+      </c>
+      <c r="X38" cm="1">
+        <f t="array" ref="X38:Z38">FIND($L$33:$N$33,W38)</f>
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <v>2</v>
+      </c>
+      <c r="Z38" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA38" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB38" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC38" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E39" t="str">
+        <v>212</v>
+      </c>
+      <c r="J39" t="str">
+        <v>122</v>
+      </c>
+      <c r="R39" t="str">
+        <v>22</v>
+      </c>
+      <c r="S39" t="str">
+        <v>221</v>
+      </c>
+      <c r="T39" t="str">
+        <v>222</v>
+      </c>
+      <c r="U39" t="str">
+        <v>223</v>
+      </c>
+      <c r="W39" t="str">
+        <v>122</v>
+      </c>
+      <c r="X39" cm="1">
+        <f t="array" ref="X39:Z39">FIND($L$33:$N$33,W39)</f>
+        <v>1</v>
+      </c>
+      <c r="Y39">
+        <v>2</v>
+      </c>
+      <c r="Z39" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA39" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB39" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC39" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E40" t="str">
+        <v>213</v>
+      </c>
+      <c r="J40" t="str">
+        <v>123</v>
+      </c>
+      <c r="R40" t="str">
+        <v>23</v>
+      </c>
+      <c r="S40" t="str">
+        <v>231</v>
+      </c>
+      <c r="T40" t="str">
+        <v>232</v>
+      </c>
+      <c r="U40" t="str">
+        <v>233</v>
+      </c>
+      <c r="W40" t="str">
+        <v>123</v>
+      </c>
+      <c r="X40" cm="1">
+        <f t="array" ref="X40:Z40">FIND($L$33:$N$33,W40)</f>
+        <v>1</v>
+      </c>
+      <c r="Y40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
+        <v>3</v>
+      </c>
+      <c r="AA40" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB40" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC40" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E41" t="str">
+        <v>221</v>
+      </c>
+      <c r="J41" t="str">
+        <v>131</v>
+      </c>
+      <c r="R41" t="str">
+        <v>31</v>
+      </c>
+      <c r="S41" t="str">
+        <v>311</v>
+      </c>
+      <c r="T41" t="str">
+        <v>312</v>
+      </c>
+      <c r="U41" t="str">
+        <v>313</v>
+      </c>
+      <c r="W41" t="str">
+        <v>131</v>
+      </c>
+      <c r="X41" cm="1">
+        <f t="array" ref="X41:Z41">FIND($L$33:$N$33,W41)</f>
+        <v>1</v>
+      </c>
+      <c r="Y41" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z41">
+        <v>2</v>
+      </c>
+      <c r="AA41" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB41" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC41" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E42" t="str">
+        <v>222</v>
+      </c>
+      <c r="J42" t="str">
+        <v>132</v>
+      </c>
+      <c r="R42" t="str">
+        <v>32</v>
+      </c>
+      <c r="S42" t="str">
+        <v>321</v>
+      </c>
+      <c r="T42" t="str">
+        <v>322</v>
+      </c>
+      <c r="U42" t="str">
+        <v>323</v>
+      </c>
+      <c r="W42" t="str">
+        <v>132</v>
+      </c>
+      <c r="X42" cm="1">
+        <f t="array" ref="X42:Z42">FIND($L$33:$N$33,W42)</f>
+        <v>1</v>
+      </c>
+      <c r="Y42">
+        <v>3</v>
+      </c>
+      <c r="Z42">
+        <v>2</v>
+      </c>
+      <c r="AA42" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB42" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC42" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E43" t="str">
+        <v>223</v>
+      </c>
+      <c r="J43" t="str">
+        <v>133</v>
+      </c>
+      <c r="R43" t="str">
+        <v>33</v>
+      </c>
+      <c r="S43" t="str">
+        <v>331</v>
+      </c>
+      <c r="T43" t="str">
+        <v>332</v>
+      </c>
+      <c r="U43" t="str">
+        <v>333</v>
+      </c>
+      <c r="W43" t="str">
+        <v>133</v>
+      </c>
+      <c r="X43" cm="1">
+        <f t="array" ref="X43:Z43">FIND($L$33:$N$33,W43)</f>
+        <v>1</v>
+      </c>
+      <c r="Y43" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z43">
+        <v>2</v>
+      </c>
+      <c r="AA43" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB43" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC43" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E44" t="str">
+        <v>231</v>
+      </c>
+      <c r="J44" t="str">
+        <v>211</v>
+      </c>
+      <c r="W44" t="str">
+        <v>211</v>
+      </c>
+      <c r="X44" cm="1">
+        <f t="array" ref="X44:Z44">FIND($L$33:$N$33,W44)</f>
+        <v>2</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+      <c r="Z44" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA44" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB44" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC44" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E45" t="str">
+        <v>232</v>
+      </c>
+      <c r="J45" t="str">
+        <v>212</v>
+      </c>
+      <c r="W45" t="str">
+        <v>212</v>
+      </c>
+      <c r="X45" cm="1">
+        <f t="array" ref="X45:Z45">FIND($L$33:$N$33,W45)</f>
+        <v>2</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="Z45" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB45" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC45" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E46" t="str">
+        <v>233</v>
+      </c>
+      <c r="J46" t="str">
+        <v>213</v>
+      </c>
+      <c r="W46" t="str">
+        <v>213</v>
+      </c>
+      <c r="X46" cm="1">
+        <f t="array" ref="X46:Z46">FIND($L$33:$N$33,W46)</f>
+        <v>2</v>
+      </c>
+      <c r="Y46">
+        <v>1</v>
+      </c>
+      <c r="Z46">
+        <v>3</v>
+      </c>
+      <c r="AA46" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB46" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC46" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E47" t="str">
+        <v>311</v>
+      </c>
+      <c r="J47" t="str">
+        <v>221</v>
+      </c>
+      <c r="W47" t="str">
+        <v>221</v>
+      </c>
+      <c r="X47" cm="1">
+        <f t="array" ref="X47:Z47">FIND($L$33:$N$33,W47)</f>
+        <v>3</v>
+      </c>
+      <c r="Y47">
+        <v>1</v>
+      </c>
+      <c r="Z47" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA47" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB47" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC47" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E48" t="str">
+        <v>312</v>
+      </c>
+      <c r="J48" t="str">
+        <v>222</v>
+      </c>
+      <c r="W48" t="str">
+        <v>222</v>
+      </c>
+      <c r="X48" t="e" cm="1">
+        <f t="array" ref="X48:Z48">FIND($L$33:$N$33,W48)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y48">
+        <v>1</v>
+      </c>
+      <c r="Z48" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB48" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC48" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E49" t="str">
+        <v>313</v>
+      </c>
+      <c r="J49" t="str">
+        <v>223</v>
+      </c>
+      <c r="W49" t="str">
+        <v>223</v>
+      </c>
+      <c r="X49" t="e" cm="1">
+        <f t="array" ref="X49:Z49">FIND($L$33:$N$33,W49)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y49">
+        <v>1</v>
+      </c>
+      <c r="Z49">
+        <v>3</v>
+      </c>
+      <c r="AA49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB49" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC49" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E50" t="str">
+        <v>321</v>
+      </c>
+      <c r="J50" t="str">
+        <v>231</v>
+      </c>
+      <c r="W50" t="str">
+        <v>231</v>
+      </c>
+      <c r="X50" cm="1">
+        <f t="array" ref="X50:Z50">FIND($L$33:$N$33,W50)</f>
+        <v>3</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50">
+        <v>2</v>
+      </c>
+      <c r="AA50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB50" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC50" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E51" t="str">
+        <v>322</v>
+      </c>
+      <c r="J51" t="str">
+        <v>232</v>
+      </c>
+      <c r="W51" t="str">
+        <v>232</v>
+      </c>
+      <c r="X51" t="e" cm="1">
+        <f t="array" ref="X51:Z51">FIND($L$33:$N$33,W51)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y51">
+        <v>1</v>
+      </c>
+      <c r="Z51">
+        <v>2</v>
+      </c>
+      <c r="AA51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB51" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC51" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E52" t="str">
+        <v>323</v>
+      </c>
+      <c r="J52" t="str">
+        <v>233</v>
+      </c>
+      <c r="W52" t="str">
+        <v>233</v>
+      </c>
+      <c r="X52" t="e" cm="1">
+        <f t="array" ref="X52:Z52">FIND($L$33:$N$33,W52)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y52">
+        <v>1</v>
+      </c>
+      <c r="Z52">
+        <v>2</v>
+      </c>
+      <c r="AA52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB52" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC52" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E53" t="str">
+        <v>331</v>
+      </c>
+      <c r="J53" t="str">
+        <v>311</v>
+      </c>
+      <c r="W53" t="str">
+        <v>311</v>
+      </c>
+      <c r="X53" cm="1">
+        <f t="array" ref="X53:Z53">FIND($L$33:$N$33,W53)</f>
+        <v>2</v>
+      </c>
+      <c r="Y53" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z53">
+        <v>1</v>
+      </c>
+      <c r="AA53" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB53" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC53" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E54" t="str">
+        <v>332</v>
+      </c>
+      <c r="J54" t="str">
+        <v>312</v>
+      </c>
+      <c r="W54" t="str">
+        <v>312</v>
+      </c>
+      <c r="X54" cm="1">
+        <f t="array" ref="X54:Z54">FIND($L$33:$N$33,W54)</f>
+        <v>2</v>
+      </c>
+      <c r="Y54">
+        <v>3</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+      <c r="AA54" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB54" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC54" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E55" t="str">
+        <v>333</v>
+      </c>
+      <c r="J55" t="str">
+        <v>313</v>
+      </c>
+      <c r="W55" t="str">
+        <v>313</v>
+      </c>
+      <c r="X55" cm="1">
+        <f t="array" ref="X55:Z55">FIND($L$33:$N$33,W55)</f>
+        <v>2</v>
+      </c>
+      <c r="Y55" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z55">
+        <v>1</v>
+      </c>
+      <c r="AA55" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB55" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC55" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J56" t="str">
+        <v>321</v>
+      </c>
+      <c r="W56" t="str">
+        <v>321</v>
+      </c>
+      <c r="X56" cm="1">
+        <f t="array" ref="X56:Z56">FIND($L$33:$N$33,W56)</f>
+        <v>3</v>
+      </c>
+      <c r="Y56">
+        <v>2</v>
+      </c>
+      <c r="Z56">
+        <v>1</v>
+      </c>
+      <c r="AA56" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB56" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC56" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J57" t="str">
+        <v>322</v>
+      </c>
+      <c r="W57" t="str">
+        <v>322</v>
+      </c>
+      <c r="X57" t="e" cm="1">
+        <f t="array" ref="X57:Z57">FIND($L$33:$N$33,W57)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y57">
+        <v>2</v>
+      </c>
+      <c r="Z57">
+        <v>1</v>
+      </c>
+      <c r="AA57" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB57" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC57" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J58" t="str">
+        <v>323</v>
+      </c>
+      <c r="W58" t="str">
+        <v>323</v>
+      </c>
+      <c r="X58" t="e" cm="1">
+        <f t="array" ref="X58:Z58">FIND($L$33:$N$33,W58)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y58">
+        <v>2</v>
+      </c>
+      <c r="Z58">
+        <v>1</v>
+      </c>
+      <c r="AA58" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB58" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC58" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J59" t="str">
+        <v>331</v>
+      </c>
+      <c r="W59" t="str">
+        <v>331</v>
+      </c>
+      <c r="X59" cm="1">
+        <f t="array" ref="X59:Z59">FIND($L$33:$N$33,W59)</f>
+        <v>3</v>
+      </c>
+      <c r="Y59" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z59">
+        <v>1</v>
+      </c>
+      <c r="AA59" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB59" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC59" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J60" t="str">
+        <v>332</v>
+      </c>
+      <c r="W60" t="str">
+        <v>332</v>
+      </c>
+      <c r="X60" t="e" cm="1">
+        <f t="array" ref="X60:Z60">FIND($L$33:$N$33,W60)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y60">
+        <v>3</v>
+      </c>
+      <c r="Z60">
+        <v>1</v>
+      </c>
+      <c r="AA60" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB60" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC60" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="J61" t="str">
+        <v>333</v>
+      </c>
+      <c r="W61" t="str">
+        <v>333</v>
+      </c>
+      <c r="X61" t="e" cm="1">
+        <f t="array" ref="X61:Z61">FIND($L$33:$N$33,W61)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y61" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z61">
+        <v>1</v>
+      </c>
+      <c r="AA61" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB61" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC61" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="W35:W61">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISNUMBER(X35),ISNUMBER(Y35),ISNUMBER(Z35))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1775,19 +2930,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="13">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1795,11 +2946,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
-        <v>2</v>
-      </c>
-      <c r="F21" s="13">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1807,19 +2957,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1827,11 +2973,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1839,19 +2984,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1859,11 +3000,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1871,13 +3011,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>